<commit_message>
Work in progress : notamment code pour tracer les résidus dans 'Modèle et Mesure'
</commit_message>
<xml_diff>
--- a/2-modèle G modifié/calibration/3_Modèle et Mesure/résultats Modèle et Mesure.xlsx
+++ b/2-modèle G modifié/calibration/3_Modèle et Mesure/résultats Modèle et Mesure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero 3A 2023-2024\projet recherche\travail concret projet\2-modèle G modifié\calibration\3_Modèle et Mesure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\2-modèle G modifié\calibration\3_Modèle et Mesure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A20CCC-C63C-4B6E-8592-792BF49F9DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDFCFA2-0250-4E06-A748-E18355B0995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implementation of alpha_var_gamma in order to compute min chi2 with modification of alpha and gamma at the same time
</commit_message>
<xml_diff>
--- a/2-modèle G modifié/calibration/3_Modèle et Mesure/résultats Modèle et Mesure.xlsx
+++ b/2-modèle G modifié/calibration/3_Modèle et Mesure/résultats Modèle et Mesure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\Desktop\Supaero_3A_2023-2024\projet_recherche\travail_concret_projet\2-modèle G modifié\calibration\3_Modèle et Mesure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDFCFA2-0250-4E06-A748-E18355B0995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7DC04A-6A3E-42C1-86D4-24893BFB684C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>alpha</t>
   </si>
@@ -503,7 +503,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +578,15 @@
         <v>16</v>
       </c>
       <c r="E2">
-        <v>4.8470000000000404</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>4.8470000000000004</v>
+      </c>
+      <c r="F2">
+        <f>ABS(E2-4.96700000000008)</f>
+        <v>0.12000000000007915</v>
+      </c>
+      <c r="G2">
+        <f>ABS(E2-4.727)</f>
+        <v>0.12000000000000011</v>
       </c>
       <c r="K2">
         <v>2168.3486379577498</v>

</xml_diff>